<commit_message>
'new ingest package fields in reader and template'
</commit_message>
<xml_diff>
--- a/avalon-csv-reader-template.xlsx
+++ b/avalon-csv-reader-template.xlsx
@@ -5,33 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry_neels/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry_neels/gbh/mlavalon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{049BDD0D-969A-E540-BF31-6F2D9A61F7B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E45A4534-359A-2146-A26B-0D206C1FF06D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{B6CD0C92-5775-3145-87B6-DE32EBBE23DA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="avalon-csv-reader-template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+  <si>
+    <t>Collection Name</t>
+  </si>
+  <si>
+    <t>Collection ID</t>
+  </si>
   <si>
     <t>Title</t>
   </si>
@@ -106,13 +101,160 @@
   </si>
   <si>
     <t>File Comment</t>
+  </si>
+  <si>
+    <t>Nova Ep 1</t>
+  </si>
+  <si>
+    <t>First Nova Episode</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Big Explosion!</t>
+  </si>
+  <si>
+    <t>nova_ep_1.mp4</t>
+  </si>
+  <si>
+    <t>nova1</t>
+  </si>
+  <si>
+    <t>https://avalon.wgbh.org/hls/avalon/baby_eleanor.mp4/master.m3u8</t>
+  </si>
+  <si>
+    <t>nova_ep_1_uncut.mp4</t>
+  </si>
+  <si>
+    <t>Nova Ep 2</t>
+  </si>
+  <si>
+    <t>Second Nova Episode</t>
+  </si>
+  <si>
+    <t>Small Explosion…</t>
+  </si>
+  <si>
+    <t>nova_ep_2_interview_outtakes.mp4</t>
+  </si>
+  <si>
+    <t>nova2</t>
+  </si>
+  <si>
+    <t>Frontline 1/4/94</t>
+  </si>
+  <si>
+    <t>Frontline from some day</t>
+  </si>
+  <si>
+    <t>Frontline</t>
+  </si>
+  <si>
+    <t>Explosions of Political Strife</t>
+  </si>
+  <si>
+    <t>frontline.mp4</t>
+  </si>
+  <si>
+    <t>frontline</t>
+  </si>
+  <si>
+    <t>frontline_deleted_scenes_and_bloopers.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Collection Description</t>
+  </si>
+  <si>
+    <t>Unit Name</t>
+  </si>
+  <si>
+    <t>Statement Of Responsibility</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Copyright Date</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Bibliographic Id</t>
+  </si>
+  <si>
+    <t>Terms Of Use</t>
+  </si>
+  <si>
+    <t>Physical Description</t>
+  </si>
+  <si>
+    <t>Creators</t>
+  </si>
+  <si>
+    <t>Alternative Titles</t>
+  </si>
+  <si>
+    <t>Translated Titles</t>
+  </si>
+  <si>
+    <t>Uniform Titles</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Resource Types</t>
+  </si>
+  <si>
+    <t>Contributors</t>
+  </si>
+  <si>
+    <t>Publishers</t>
+  </si>
+  <si>
+    <t>Genres</t>
+  </si>
+  <si>
+    <t>Subjects</t>
+  </si>
+  <si>
+    <t>Related Item Urls</t>
+  </si>
+  <si>
+    <t>Geographic Subjects</t>
+  </si>
+  <si>
+    <t>Temporal Subjects</t>
+  </si>
+  <si>
+    <t>Topical Subjects</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Tables Of Contents</t>
+  </si>
+  <si>
+    <t>Other Identifiers</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,16 +262,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -137,15 +579,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -456,91 +1088,360 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD8B6A1-318F-344D-AF5A-0C5FFE86E31F}">
-  <dimension ref="A1:Y1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BC11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AH1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AI1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AJ1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AK1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AL1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AM1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AN1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AO1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AP1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AQ1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AR1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AS1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AT1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AU1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AV1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AW1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AX1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AY1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AZ1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="BA1" t="s">
         <v>24</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1">
+        <v>36526</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1">
+        <v>36526</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ4">
+        <v>2</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1">
+        <v>36557</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6">
+        <v>3</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1">
+        <v>36557</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ7">
+        <v>4</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1">
+        <v>36586</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ9">
+        <v>5</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1">
+        <v>36586</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ10">
+        <v>6</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>